<commit_message>
change structure excell(hat), add inv,agregat to transportExcell, sorted by type_of_work, CHANGE ALGORITM OF DRIWING
</commit_message>
<xml_diff>
--- a/config/config.xlsx
+++ b/config/config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
   </bookViews>
   <sheets>
     <sheet name="combaine" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="174">
   <si>
     <t>Марка ТЗ</t>
   </si>
@@ -504,6 +504,42 @@
   </si>
   <si>
     <t>копання картоплі</t>
+  </si>
+  <si>
+    <t>Роїще</t>
+  </si>
+  <si>
+    <t>Ро</t>
+  </si>
+  <si>
+    <t>Новий Білоус</t>
+  </si>
+  <si>
+    <t>НБ</t>
+  </si>
+  <si>
+    <t>Рудка</t>
+  </si>
+  <si>
+    <t>Ру</t>
+  </si>
+  <si>
+    <t>Пльохів</t>
+  </si>
+  <si>
+    <t>Пл</t>
+  </si>
+  <si>
+    <t>Жукотки</t>
+  </si>
+  <si>
+    <t>Жу</t>
+  </si>
+  <si>
+    <t>Велика Вісь</t>
+  </si>
+  <si>
+    <t>ВВ</t>
   </si>
 </sst>
 </file>
@@ -1140,8 +1176,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,10 +1404,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,6 +1470,54 @@
       </c>
       <c r="B7" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>168</v>
+      </c>
+      <c r="B11" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B13" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1646,8 +1730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>